<commit_message>
Added logos to all sheets
</commit_message>
<xml_diff>
--- a/jump.xlsx
+++ b/jump.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedove\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PederHans\code\divesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -254,7 +254,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1345,7 +1345,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -1577,319 +1577,313 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="7" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="7" fillId="0" borderId="46" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="70" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="70" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="7" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="7" fillId="0" borderId="46" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1977,6 +1971,161 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>347264</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>217715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE14DD29-89A4-41F2-ABC5-0955A7436EE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="136071" y="340179"/>
+          <a:ext cx="1830443" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>625929</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>589372</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>265824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0445E3E5-AB48-40C9-BE4A-11001EBE586A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11933465" y="285750"/>
+          <a:ext cx="602978" cy="674038"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>421820</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>51456</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>607023</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>148755</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C299C93-5312-41C7-87A8-4F35F8383CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8313963" y="7943599"/>
+          <a:ext cx="4240131" cy="614370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2306,11 +2455,11 @@
   </sheetPr>
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="75" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="5.25" style="2" customWidth="1"/>
@@ -2327,92 +2476,92 @@
     <col min="21" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="12" customHeight="1">
+    <row r="1" spans="1:33" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:33" ht="7.15" customHeight="1">
+    <row r="2" spans="1:33" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:33" ht="36" customHeight="1">
-      <c r="A3" s="91" t="s">
+    <row r="3" spans="1:33" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="190" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="90"/>
-      <c r="T3" s="90"/>
-    </row>
-    <row r="4" spans="1:33" ht="22.15" customHeight="1">
-      <c r="A4" s="109" t="s">
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="190"/>
+      <c r="L3" s="190"/>
+      <c r="M3" s="190"/>
+      <c r="N3" s="190"/>
+      <c r="O3" s="190"/>
+      <c r="P3" s="190"/>
+      <c r="Q3" s="190"/>
+      <c r="R3" s="190"/>
+      <c r="S3" s="190"/>
+      <c r="T3" s="190"/>
+    </row>
+    <row r="4" spans="1:33" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="191" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-    </row>
-    <row r="5" spans="1:33" ht="13.15" customHeight="1">
+      <c r="B4" s="191"/>
+      <c r="C4" s="191"/>
+      <c r="D4" s="191"/>
+      <c r="E4" s="191"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="191"/>
+      <c r="H4" s="191"/>
+      <c r="I4" s="191"/>
+      <c r="J4" s="191"/>
+      <c r="K4" s="191"/>
+      <c r="L4" s="191"/>
+      <c r="M4" s="191"/>
+      <c r="N4" s="191"/>
+      <c r="O4" s="191"/>
+      <c r="P4" s="191"/>
+      <c r="Q4" s="191"/>
+      <c r="R4" s="191"/>
+      <c r="S4" s="191"/>
+      <c r="T4" s="191"/>
+    </row>
+    <row r="5" spans="1:33" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="167"/>
-      <c r="R5" s="168"/>
-      <c r="S5" s="168"/>
-      <c r="T5" s="168"/>
-    </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1">
-      <c r="A6" s="133" t="s">
+      <c r="Q5" s="90"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+    </row>
+    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="133"/>
-      <c r="C6" s="133"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="107" t="s">
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="107"/>
-      <c r="J6" s="107"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
       <c r="K6"/>
-      <c r="L6" s="107" t="s">
+      <c r="L6" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="108"/>
+      <c r="M6" s="168"/>
       <c r="N6" s="4" t="s">
         <v>32</v>
       </c>
@@ -2420,12 +2569,12 @@
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
     </row>
-    <row r="7" spans="1:33" ht="19.899999999999999" customHeight="1">
-      <c r="A7" s="125"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="127"/>
+    <row r="7" spans="1:33" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="93"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="28"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
@@ -2443,7 +2592,7 @@
       <c r="S7"/>
       <c r="T7"/>
     </row>
-    <row r="8" spans="1:33" ht="4.1500000000000004" customHeight="1">
+    <row r="8" spans="1:33" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2475,33 +2624,33 @@
       <c r="AF8" s="10"/>
       <c r="AG8" s="10"/>
     </row>
-    <row r="9" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="A9" s="133" t="s">
+    <row r="9" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="133"/>
-      <c r="C9" s="133"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="107" t="s">
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="107"/>
-      <c r="J9" s="107"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
       <c r="K9"/>
-      <c r="L9" s="107" t="s">
+      <c r="L9" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="108"/>
+      <c r="M9" s="168"/>
       <c r="N9" s="4" t="s">
         <v>32</v>
       </c>
       <c r="O9"/>
       <c r="P9"/>
-      <c r="Q9" s="143"/>
-      <c r="R9" s="143"/>
+      <c r="Q9" s="167"/>
+      <c r="R9" s="167"/>
       <c r="S9"/>
       <c r="T9"/>
       <c r="U9" s="13"/>
@@ -2513,12 +2662,12 @@
       <c r="AF9" s="16"/>
       <c r="AG9" s="17"/>
     </row>
-    <row r="10" spans="1:33" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="A10" s="125"/>
-      <c r="B10" s="126"/>
-      <c r="C10" s="126"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="127"/>
+    <row r="10" spans="1:33" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="93"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
       <c r="F10" s="28"/>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
@@ -2550,7 +2699,7 @@
       <c r="AF10" s="20"/>
       <c r="AG10" s="20"/>
     </row>
-    <row r="11" spans="1:33" ht="4.9000000000000004" customHeight="1" thickBot="1">
+    <row r="11" spans="1:33" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -2583,26 +2732,26 @@
       <c r="AF11" s="20"/>
       <c r="AG11" s="20"/>
     </row>
-    <row r="12" spans="1:33" ht="15" customHeight="1" thickTop="1">
-      <c r="A12" s="133" t="s">
+    <row r="12" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="107" t="s">
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="107"/>
-      <c r="J12" s="107"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="107" t="s">
+      <c r="L12" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="M12" s="108"/>
+      <c r="M12" s="168"/>
       <c r="N12" s="4" t="s">
         <v>32</v>
       </c>
@@ -2624,12 +2773,12 @@
       <c r="AF12" s="20"/>
       <c r="AG12" s="20"/>
     </row>
-    <row r="13" spans="1:33" ht="19.899999999999999" customHeight="1">
-      <c r="A13" s="180"/>
-      <c r="B13" s="181"/>
-      <c r="C13" s="181"/>
-      <c r="D13" s="181"/>
-      <c r="E13" s="182"/>
+    <row r="13" spans="1:33" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="107"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="109"/>
       <c r="F13" s="70"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
@@ -2661,7 +2810,7 @@
       <c r="AF13" s="20"/>
       <c r="AG13" s="20"/>
     </row>
-    <row r="14" spans="1:33" ht="4.9000000000000004" customHeight="1">
+    <row r="14" spans="1:33" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
@@ -2694,26 +2843,26 @@
       <c r="AF14" s="20"/>
       <c r="AG14" s="20"/>
     </row>
-    <row r="15" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="A15" s="133" t="s">
+    <row r="15" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="133"/>
-      <c r="C15" s="133"/>
-      <c r="D15" s="133"/>
-      <c r="E15" s="133"/>
-      <c r="F15" s="133"/>
-      <c r="G15" s="133"/>
-      <c r="H15" s="107" t="s">
+      <c r="B15" s="92"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="107"/>
-      <c r="J15" s="107"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="107" t="s">
+      <c r="L15" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="108"/>
+      <c r="M15" s="168"/>
       <c r="N15" s="4" t="s">
         <v>32</v>
       </c>
@@ -2735,12 +2884,12 @@
       <c r="AF15" s="20"/>
       <c r="AG15" s="20"/>
     </row>
-    <row r="16" spans="1:33" ht="19.899999999999999" customHeight="1">
-      <c r="A16" s="180"/>
-      <c r="B16" s="181"/>
-      <c r="C16" s="181"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="182"/>
+    <row r="16" spans="1:33" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="107"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="109"/>
       <c r="F16" s="70"/>
       <c r="G16" s="6"/>
       <c r="H16" s="7"/>
@@ -2756,8 +2905,8 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
-      <c r="S16" s="137"/>
-      <c r="T16" s="138"/>
+      <c r="S16" s="161"/>
+      <c r="T16" s="162"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
       <c r="W16" s="4"/>
@@ -2770,7 +2919,7 @@
       <c r="AF16" s="20"/>
       <c r="AG16" s="20"/>
     </row>
-    <row r="17" spans="1:33" ht="28.15" customHeight="1" thickBot="1">
+    <row r="17" spans="1:33" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -2789,8 +2938,8 @@
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
-      <c r="S17" s="139"/>
-      <c r="T17" s="140"/>
+      <c r="S17" s="163"/>
+      <c r="T17" s="164"/>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
       <c r="W17" s="13"/>
@@ -2803,35 +2952,35 @@
       <c r="AF17" s="21"/>
       <c r="AG17" s="15"/>
     </row>
-    <row r="18" spans="1:33" ht="16.149999999999999" customHeight="1" thickBot="1">
-      <c r="A18" s="128" t="s">
+    <row r="18" spans="1:33" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="153" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="130"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="131"/>
-      <c r="J18" s="128" t="s">
+      <c r="B18" s="154"/>
+      <c r="C18" s="154"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="155"/>
+      <c r="F18" s="155"/>
+      <c r="G18" s="155"/>
+      <c r="H18" s="155"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="153" t="s">
         <v>4</v>
       </c>
-      <c r="K18" s="130"/>
-      <c r="L18" s="130"/>
-      <c r="M18" s="130"/>
-      <c r="N18" s="132"/>
+      <c r="K18" s="155"/>
+      <c r="L18" s="155"/>
+      <c r="M18" s="155"/>
+      <c r="N18" s="157"/>
       <c r="O18" s="68"/>
-      <c r="P18" s="134" t="s">
+      <c r="P18" s="158" t="s">
         <v>24</v>
       </c>
-      <c r="Q18" s="135"/>
-      <c r="R18" s="136"/>
-      <c r="S18" s="141"/>
-      <c r="T18" s="142"/>
-    </row>
-    <row r="19" spans="1:33" ht="28.15" customHeight="1" thickBot="1">
+      <c r="Q18" s="159"/>
+      <c r="R18" s="160"/>
+      <c r="S18" s="165"/>
+      <c r="T18" s="166"/>
+    </row>
+    <row r="19" spans="1:33" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>5</v>
       </c>
@@ -2877,289 +3026,289 @@
       <c r="O19" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="189" t="s">
+      <c r="P19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="Q19" s="190"/>
-      <c r="R19" s="190"/>
-      <c r="S19" s="190"/>
-      <c r="T19" s="191"/>
-    </row>
-    <row r="20" spans="1:33" ht="24" customHeight="1">
+      <c r="Q19" s="121"/>
+      <c r="R19" s="121"/>
+      <c r="S19" s="121"/>
+      <c r="T19" s="122"/>
+    </row>
+    <row r="20" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="50" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="56"/>
-      <c r="C20" s="104" t="s">
+      <c r="C20" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="101">
+      <c r="D20" s="127">
         <v>1</v>
       </c>
-      <c r="E20" s="93" t="s">
+      <c r="E20" s="185" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="192" t="s">
+      <c r="F20" s="137"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="164"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="99"/>
-      <c r="M20" s="99"/>
-      <c r="N20" s="99"/>
-      <c r="O20" s="101"/>
+      <c r="I20" s="139"/>
+      <c r="J20" s="185"/>
+      <c r="K20" s="137"/>
+      <c r="L20" s="137"/>
+      <c r="M20" s="137"/>
+      <c r="N20" s="137"/>
+      <c r="O20" s="127"/>
       <c r="P20" s="51"/>
       <c r="Q20" s="52"/>
       <c r="R20" s="57"/>
       <c r="S20" s="51"/>
       <c r="T20" s="53"/>
     </row>
-    <row r="21" spans="1:33" ht="24" customHeight="1" thickBot="1">
+    <row r="21" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="54" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="55"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="116"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="165"/>
-      <c r="J21" s="103"/>
-      <c r="K21" s="100"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="100"/>
-      <c r="N21" s="100"/>
-      <c r="O21" s="102"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="186"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="140"/>
+      <c r="J21" s="187"/>
+      <c r="K21" s="141"/>
+      <c r="L21" s="141"/>
+      <c r="M21" s="141"/>
+      <c r="N21" s="141"/>
+      <c r="O21" s="128"/>
       <c r="P21" s="63"/>
       <c r="Q21" s="64"/>
       <c r="R21" s="65"/>
       <c r="S21" s="66"/>
       <c r="T21" s="67"/>
     </row>
-    <row r="22" spans="1:33" ht="24" customHeight="1" thickBot="1">
-      <c r="A22" s="110" t="s">
+    <row r="22" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="114"/>
-      <c r="C22" s="104" t="s">
+      <c r="B22" s="183"/>
+      <c r="C22" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="101">
+      <c r="D22" s="127">
         <v>2</v>
       </c>
-      <c r="E22" s="93" t="s">
+      <c r="E22" s="185" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="99"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="99" t="s">
+      <c r="F22" s="137"/>
+      <c r="G22" s="137"/>
+      <c r="H22" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="101"/>
-      <c r="J22" s="93"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="99"/>
-      <c r="M22" s="99"/>
-      <c r="N22" s="99"/>
-      <c r="O22" s="101"/>
+      <c r="I22" s="127"/>
+      <c r="J22" s="185"/>
+      <c r="K22" s="137"/>
+      <c r="L22" s="137"/>
+      <c r="M22" s="137"/>
+      <c r="N22" s="137"/>
+      <c r="O22" s="127"/>
       <c r="P22" s="78"/>
       <c r="Q22" s="79"/>
       <c r="R22" s="80"/>
       <c r="S22" s="78"/>
       <c r="T22" s="80"/>
     </row>
-    <row r="23" spans="1:33" ht="24" customHeight="1" thickBot="1">
-      <c r="A23" s="111"/>
-      <c r="B23" s="115"/>
-      <c r="C23" s="112"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="113"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="116"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="116"/>
-      <c r="N23" s="116"/>
-      <c r="O23" s="113"/>
+    <row r="23" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="180"/>
+      <c r="B23" s="184"/>
+      <c r="C23" s="181"/>
+      <c r="D23" s="182"/>
+      <c r="E23" s="186"/>
+      <c r="F23" s="138"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="138"/>
+      <c r="I23" s="182"/>
+      <c r="J23" s="186"/>
+      <c r="K23" s="138"/>
+      <c r="L23" s="138"/>
+      <c r="M23" s="138"/>
+      <c r="N23" s="138"/>
+      <c r="O23" s="182"/>
       <c r="P23" s="85"/>
       <c r="Q23" s="85"/>
       <c r="R23" s="86"/>
       <c r="S23" s="85"/>
       <c r="T23" s="86"/>
     </row>
-    <row r="24" spans="1:33" ht="24" customHeight="1">
+    <row r="24" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="62" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="56"/>
-      <c r="C24" s="183" t="s">
+      <c r="C24" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="185">
+      <c r="D24" s="112">
         <v>3</v>
       </c>
-      <c r="E24" s="95" t="s">
+      <c r="E24" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="150"/>
-      <c r="G24" s="150"/>
-      <c r="H24" s="150" t="s">
+      <c r="F24" s="114"/>
+      <c r="G24" s="114"/>
+      <c r="H24" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="187"/>
-      <c r="J24" s="95"/>
-      <c r="K24" s="150"/>
-      <c r="L24" s="150"/>
-      <c r="M24" s="150"/>
-      <c r="N24" s="150"/>
-      <c r="O24" s="185"/>
+      <c r="I24" s="116"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="114"/>
+      <c r="L24" s="114"/>
+      <c r="M24" s="114"/>
+      <c r="N24" s="114"/>
+      <c r="O24" s="112"/>
       <c r="P24" s="83"/>
       <c r="Q24" s="83"/>
       <c r="R24" s="84"/>
       <c r="S24" s="83"/>
       <c r="T24" s="84"/>
     </row>
-    <row r="25" spans="1:33" ht="24" customHeight="1" thickBot="1">
+    <row r="25" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="61"/>
-      <c r="C25" s="184"/>
-      <c r="D25" s="186"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="151"/>
-      <c r="G25" s="151"/>
-      <c r="H25" s="151"/>
-      <c r="I25" s="188"/>
-      <c r="J25" s="96"/>
-      <c r="K25" s="151"/>
-      <c r="L25" s="151"/>
-      <c r="M25" s="151"/>
-      <c r="N25" s="151"/>
-      <c r="O25" s="186"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="119"/>
+      <c r="K25" s="115"/>
+      <c r="L25" s="115"/>
+      <c r="M25" s="115"/>
+      <c r="N25" s="115"/>
+      <c r="O25" s="113"/>
       <c r="P25" s="87"/>
       <c r="Q25" s="87"/>
       <c r="R25" s="88"/>
       <c r="S25" s="87"/>
       <c r="T25" s="88"/>
     </row>
-    <row r="26" spans="1:33" ht="24" customHeight="1" thickBot="1">
-      <c r="A26" s="110" t="s">
+    <row r="26" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="146"/>
-      <c r="C26" s="104" t="s">
+      <c r="B26" s="172"/>
+      <c r="C26" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="101">
+      <c r="D26" s="127">
         <v>4</v>
       </c>
-      <c r="E26" s="93" t="s">
+      <c r="E26" s="185" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="99" t="s">
+      <c r="F26" s="137"/>
+      <c r="G26" s="137"/>
+      <c r="H26" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="101"/>
-      <c r="J26" s="93"/>
-      <c r="K26" s="99"/>
-      <c r="L26" s="99"/>
-      <c r="M26" s="99"/>
-      <c r="N26" s="99"/>
-      <c r="O26" s="101"/>
+      <c r="I26" s="127"/>
+      <c r="J26" s="185"/>
+      <c r="K26" s="137"/>
+      <c r="L26" s="137"/>
+      <c r="M26" s="137"/>
+      <c r="N26" s="137"/>
+      <c r="O26" s="127"/>
       <c r="P26" s="78"/>
       <c r="Q26" s="79"/>
       <c r="R26" s="80"/>
       <c r="S26" s="78"/>
       <c r="T26" s="80"/>
     </row>
-    <row r="27" spans="1:33" ht="24" customHeight="1" thickBot="1">
-      <c r="A27" s="144"/>
-      <c r="B27" s="147"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="103"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="100"/>
-      <c r="H27" s="100"/>
-      <c r="I27" s="102"/>
-      <c r="J27" s="103"/>
-      <c r="K27" s="100"/>
-      <c r="L27" s="100"/>
-      <c r="M27" s="100"/>
-      <c r="N27" s="100"/>
-      <c r="O27" s="102"/>
+    <row r="27" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="170"/>
+      <c r="B27" s="173"/>
+      <c r="C27" s="126"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="187"/>
+      <c r="F27" s="141"/>
+      <c r="G27" s="141"/>
+      <c r="H27" s="141"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="187"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="141"/>
+      <c r="M27" s="141"/>
+      <c r="N27" s="141"/>
+      <c r="O27" s="128"/>
       <c r="P27" s="74"/>
       <c r="Q27" s="75"/>
       <c r="R27" s="76"/>
       <c r="S27" s="77"/>
       <c r="T27" s="76"/>
     </row>
-    <row r="28" spans="1:33" ht="24" customHeight="1" thickBot="1">
-      <c r="A28" s="145" t="s">
+    <row r="28" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="148"/>
-      <c r="C28" s="149" t="s">
+      <c r="B28" s="174"/>
+      <c r="C28" s="175" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="98">
+      <c r="D28" s="189">
         <v>5</v>
       </c>
-      <c r="E28" s="106" t="s">
+      <c r="E28" s="144" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="97"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="97" t="s">
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="166"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="97"/>
-      <c r="L28" s="97"/>
-      <c r="M28" s="97"/>
-      <c r="N28" s="97"/>
-      <c r="O28" s="98"/>
+      <c r="I28" s="143"/>
+      <c r="J28" s="144"/>
+      <c r="K28" s="142"/>
+      <c r="L28" s="142"/>
+      <c r="M28" s="142"/>
+      <c r="N28" s="142"/>
+      <c r="O28" s="189"/>
       <c r="P28" s="78"/>
       <c r="Q28" s="79"/>
       <c r="R28" s="80"/>
       <c r="S28" s="81"/>
       <c r="T28" s="80"/>
     </row>
-    <row r="29" spans="1:33" ht="24" customHeight="1">
-      <c r="A29" s="145"/>
-      <c r="B29" s="148"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="166"/>
-      <c r="J29" s="106"/>
-      <c r="K29" s="97"/>
-      <c r="L29" s="97"/>
-      <c r="M29" s="97"/>
-      <c r="N29" s="97"/>
-      <c r="O29" s="98"/>
-      <c r="P29" s="169"/>
-      <c r="Q29" s="172"/>
-      <c r="R29" s="175"/>
-      <c r="S29" s="169"/>
-      <c r="T29" s="175"/>
-    </row>
-    <row r="30" spans="1:33" ht="4.9000000000000004" customHeight="1">
+    <row r="29" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="171"/>
+      <c r="B29" s="174"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="189"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="142"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="142"/>
+      <c r="I29" s="143"/>
+      <c r="J29" s="144"/>
+      <c r="K29" s="142"/>
+      <c r="L29" s="142"/>
+      <c r="M29" s="142"/>
+      <c r="N29" s="142"/>
+      <c r="O29" s="189"/>
+      <c r="P29" s="96"/>
+      <c r="Q29" s="99"/>
+      <c r="R29" s="102"/>
+      <c r="S29" s="96"/>
+      <c r="T29" s="102"/>
+    </row>
+    <row r="30" spans="1:33" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="72"/>
       <c r="B30" s="73"/>
       <c r="C30" s="73"/>
@@ -3173,141 +3322,229 @@
       <c r="K30" s="73"/>
       <c r="L30" s="73"/>
       <c r="M30" s="73"/>
-      <c r="N30" s="160" t="s">
+      <c r="N30" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="161"/>
-      <c r="P30" s="170"/>
-      <c r="Q30" s="173"/>
-      <c r="R30" s="176"/>
-      <c r="S30" s="170"/>
-      <c r="T30" s="176"/>
-    </row>
-    <row r="31" spans="1:33" ht="13.9" customHeight="1" thickBot="1">
-      <c r="A31" s="154" t="s">
+      <c r="O30" s="134"/>
+      <c r="P30" s="97"/>
+      <c r="Q30" s="100"/>
+      <c r="R30" s="103"/>
+      <c r="S30" s="97"/>
+      <c r="T30" s="103"/>
+    </row>
+    <row r="31" spans="1:33" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="155"/>
-      <c r="C31" s="155"/>
-      <c r="D31" s="155"/>
-      <c r="E31" s="155"/>
-      <c r="F31" s="155"/>
-      <c r="G31" s="155"/>
-      <c r="H31" s="155"/>
-      <c r="I31" s="155"/>
-      <c r="J31" s="155"/>
-      <c r="K31" s="155"/>
-      <c r="L31" s="155"/>
-      <c r="M31" s="155"/>
-      <c r="N31" s="162"/>
-      <c r="O31" s="163"/>
-      <c r="P31" s="171"/>
-      <c r="Q31" s="174"/>
-      <c r="R31" s="177"/>
-      <c r="S31" s="178"/>
-      <c r="T31" s="179"/>
-    </row>
-    <row r="32" spans="1:33" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="A32" s="156" t="s">
+      <c r="B31" s="179"/>
+      <c r="C31" s="179"/>
+      <c r="D31" s="179"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="179"/>
+      <c r="H31" s="179"/>
+      <c r="I31" s="179"/>
+      <c r="J31" s="179"/>
+      <c r="K31" s="179"/>
+      <c r="L31" s="179"/>
+      <c r="M31" s="179"/>
+      <c r="N31" s="135"/>
+      <c r="O31" s="136"/>
+      <c r="P31" s="98"/>
+      <c r="Q31" s="101"/>
+      <c r="R31" s="104"/>
+      <c r="S31" s="105"/>
+      <c r="T31" s="106"/>
+    </row>
+    <row r="32" spans="1:33" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="157"/>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="157"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="158"/>
-      <c r="H32" s="159" t="s">
+      <c r="B32" s="130"/>
+      <c r="C32" s="130"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="130"/>
+      <c r="F32" s="130"/>
+      <c r="G32" s="131"/>
+      <c r="H32" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="157"/>
-      <c r="J32" s="157"/>
-      <c r="K32" s="157"/>
-      <c r="L32" s="157"/>
-      <c r="M32" s="157"/>
-      <c r="N32" s="157"/>
+      <c r="I32" s="130"/>
+      <c r="J32" s="130"/>
+      <c r="K32" s="130"/>
+      <c r="L32" s="130"/>
+      <c r="M32" s="130"/>
+      <c r="N32" s="130"/>
       <c r="O32" s="44" t="s">
         <v>22</v>
       </c>
       <c r="P32" s="43"/>
       <c r="Q32" s="43"/>
       <c r="R32" s="43"/>
-      <c r="S32" s="119"/>
-      <c r="T32" s="120"/>
-    </row>
-    <row r="33" spans="1:20" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A33" s="156" t="s">
+      <c r="S32" s="147"/>
+      <c r="T32" s="148"/>
+    </row>
+    <row r="33" spans="1:20" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="158"/>
-      <c r="H33" s="159" t="s">
+      <c r="B33" s="130"/>
+      <c r="C33" s="130"/>
+      <c r="D33" s="130"/>
+      <c r="E33" s="130"/>
+      <c r="F33" s="130"/>
+      <c r="G33" s="131"/>
+      <c r="H33" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="I33" s="157"/>
-      <c r="J33" s="157"/>
-      <c r="K33" s="157"/>
-      <c r="L33" s="157"/>
-      <c r="M33" s="157"/>
-      <c r="N33" s="157"/>
+      <c r="I33" s="130"/>
+      <c r="J33" s="130"/>
+      <c r="K33" s="130"/>
+      <c r="L33" s="130"/>
+      <c r="M33" s="130"/>
+      <c r="N33" s="130"/>
       <c r="O33" s="45"/>
       <c r="P33" s="43"/>
       <c r="Q33" s="43"/>
       <c r="R33" s="43"/>
-      <c r="S33" s="121"/>
-      <c r="T33" s="122"/>
-    </row>
-    <row r="34" spans="1:20" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="152" t="s">
+      <c r="S33" s="149"/>
+      <c r="T33" s="150"/>
+    </row>
+    <row r="34" spans="1:20" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="176" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="153"/>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="123"/>
-      <c r="J34" s="123"/>
-      <c r="K34" s="123"/>
-      <c r="L34" s="123"/>
-      <c r="M34" s="123"/>
-      <c r="N34" s="124"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="177"/>
+      <c r="H34" s="151"/>
+      <c r="I34" s="151"/>
+      <c r="J34" s="151"/>
+      <c r="K34" s="151"/>
+      <c r="L34" s="151"/>
+      <c r="M34" s="151"/>
+      <c r="N34" s="152"/>
       <c r="O34" s="42"/>
       <c r="P34" s="41"/>
       <c r="Q34" s="41"/>
       <c r="R34" s="41"/>
-      <c r="S34" s="117" t="s">
+      <c r="S34" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="T34" s="118"/>
-    </row>
-    <row r="35" spans="1:20" ht="7.9" customHeight="1">
+      <c r="T34" s="146"/>
+    </row>
+    <row r="35" spans="1:20" ht="7.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="47"/>
     </row>
-    <row r="36" spans="1:20" ht="13.15" customHeight="1">
-      <c r="A36" s="92" t="s">
+    <row r="36" spans="1:20" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="92"/>
+      <c r="B36" s="188"/>
       <c r="C36" s="69" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="15">
-      <c r="A37" s="92"/>
-      <c r="B37" s="92"/>
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="188"/>
+      <c r="B37" s="188"/>
       <c r="C37" s="82" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="A3:T3"/>
+    <mergeCell ref="A4:T4"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="S32:T33"/>
+    <mergeCell ref="H34:N34"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="S16:T18"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="H32:N32"/>
+    <mergeCell ref="H33:N33"/>
+    <mergeCell ref="N30:O31"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="Q5:T5"/>
     <mergeCell ref="A6:G6"/>
@@ -3332,99 +3569,12 @@
     <mergeCell ref="O24:O25"/>
     <mergeCell ref="P19:T19"/>
     <mergeCell ref="H20:H21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="H32:N32"/>
-    <mergeCell ref="H33:N33"/>
-    <mergeCell ref="N30:O31"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="S32:T33"/>
-    <mergeCell ref="H34:N34"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S16:T18"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A31:M31"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.15375" right="0" top="0.21" bottom="0.21" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="83" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="82" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>

</xml_diff>